<commit_message>
file updation in excel sheet for reading from excel sheet
</commit_message>
<xml_diff>
--- a/src/test/java/dataEngine/dataSheet.xlsx
+++ b/src/test/java/dataEngine/dataSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rais\git\goodman-mfg\src\test\java\dataEngine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\goodman-mfg\src\test\java\dataEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="31">
   <si>
     <t>I am a(n)</t>
   </si>
@@ -99,6 +99,24 @@
   </si>
   <si>
     <t>Softway23</t>
+  </si>
+  <si>
+    <t>Softway21</t>
+  </si>
+  <si>
+    <t>Softway26</t>
+  </si>
+  <si>
+    <t>Softway25</t>
+  </si>
+  <si>
+    <t>Developer</t>
+  </si>
+  <si>
+    <t>Homeowner</t>
+  </si>
+  <si>
+    <t>HVAC Dealer</t>
   </si>
 </sst>
 </file>
@@ -436,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R2"/>
+  <dimension ref="B1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,6 +574,165 @@
         <v>23</v>
       </c>
     </row>
+    <row r="3" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="4">
+        <v>78479</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1234567895</v>
+      </c>
+      <c r="M3" s="4">
+        <v>1234567890</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K4" s="4">
+        <v>78479</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1234567895</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1234567890</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K5" s="4">
+        <v>78479</v>
+      </c>
+      <c r="L5" s="4">
+        <v>1234567895</v>
+      </c>
+      <c r="M5" s="4">
+        <v>1234567890</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changes  done for the contact us page
</commit_message>
<xml_diff>
--- a/src/test/java/dataEngine/dataSheet.xlsx
+++ b/src/test/java/dataEngine/dataSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\goodman-mfg\src\test\java\dataEngine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rais\git\goodman-mfg\src\test\java\dataEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
   <si>
     <t>I am a(n)</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Softway23</t>
   </si>
   <si>
-    <t>Softway21</t>
-  </si>
-  <si>
     <t>Softway26</t>
   </si>
   <si>
@@ -117,6 +114,24 @@
   </si>
   <si>
     <t>HVAC Dealer</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>softway</t>
+  </si>
+  <si>
+    <t>rais</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -454,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:R5"/>
+  <dimension ref="B1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +483,7 @@
     <col min="14" max="16384" width="12.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,8 +535,11 @@
       <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="S1" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="2" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
@@ -573,13 +591,16 @@
       <c r="R2" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="S2" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="3" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>18</v>
@@ -603,13 +624,13 @@
         <v>20</v>
       </c>
       <c r="K3" s="4">
-        <v>78479</v>
+        <v>123456</v>
       </c>
       <c r="L3" s="4">
-        <v>1234567895</v>
-      </c>
-      <c r="M3" s="4">
-        <v>1234567890</v>
+        <v>12345645454</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="N3" s="2" t="s">
         <v>21</v>
@@ -626,13 +647,16 @@
       <c r="R3" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="S3" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="4" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>18</v>
@@ -679,13 +703,16 @@
       <c r="R4" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="S4" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="5" spans="2:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>18</v>
@@ -718,7 +745,7 @@
         <v>1234567890</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>18</v>
@@ -731,6 +758,9 @@
       </c>
       <c r="R5" s="2" t="s">
         <v>23</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated and crearted the Test case Product page
</commit_message>
<xml_diff>
--- a/src/test/java/dataEngine/dataSheet.xlsx
+++ b/src/test/java/dataEngine/dataSheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
   <si>
     <t>I am a(n)</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>soft</t>
   </si>
 </sst>
 </file>
@@ -596,6 +599,9 @@
       <c r="B3" t="s">
         <v>27</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="D3" s="2" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Wrote Test Cases for Products and Product Details pages.
</commit_message>
<xml_diff>
--- a/src/test/java/dataEngine/dataSheet.xlsx
+++ b/src/test/java/dataEngine/dataSheet.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\goodman-mfg\src\test\java\dataEngine\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ContactUs" sheetId="1" r:id="rId1"/>
+    <sheet name="ProductEmail" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="43">
   <si>
     <t>I am a(n)</t>
   </si>
@@ -132,13 +128,34 @@
   </si>
   <si>
     <t>soft</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>raees@softway.com</t>
+  </si>
+  <si>
+    <t>This is a test message…</t>
+  </si>
+  <si>
+    <t>This is a test message2…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +167,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -172,10 +197,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -189,8 +215,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -249,7 +278,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -284,7 +313,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -461,7 +490,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -471,7 +500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -767,4 +796,74 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added test cases and logic for Product Details and Product Category pages
</commit_message>
<xml_diff>
--- a/src/test/java/dataEngine/dataSheet.xlsx
+++ b/src/test/java/dataEngine/dataSheet.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rais\git\goodman-mfg\src\test\java\dataEngine\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9735" activeTab="1"/>
   </bookViews>
@@ -20,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
   <si>
     <t>I am a(n)</t>
   </si>
@@ -149,6 +154,9 @@
   </si>
   <si>
     <t>This is a test message2…</t>
+  </si>
+  <si>
+    <t>Test2</t>
   </si>
 </sst>
 </file>
@@ -490,7 +498,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -803,7 +811,7 @@
   <dimension ref="B1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,7 +858,7 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
         <v>42</v>
@@ -864,6 +872,6 @@
     <hyperlink ref="C3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>